<commit_message>
Skelleton of reservation conflict check
</commit_message>
<xml_diff>
--- a/public/spreadsheets/horarios.xlsx
+++ b/public/spreadsheets/horarios.xlsx
@@ -434,42 +434,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection hidden="1"/>
     </xf>
@@ -489,6 +453,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -498,8 +465,41 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -800,382 +800,382 @@
   <dimension ref="A1:O14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" style="21" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="30.5" style="21" customWidth="1"/>
-    <col min="4" max="4" width="11" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="36" style="21" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5" style="21" customWidth="1"/>
-    <col min="8" max="8" width="61.83203125" style="21" customWidth="1"/>
-    <col min="9" max="9" width="34.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="44.1640625" style="21" customWidth="1"/>
-    <col min="11" max="11" width="15.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.5" style="21" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="16.83203125" style="21" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="37" style="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="16384" width="8.83203125" style="21"/>
+    <col min="1" max="1" width="11.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="30.5" style="9" customWidth="1"/>
+    <col min="4" max="4" width="11" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="36" style="9" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5" style="9" customWidth="1"/>
+    <col min="8" max="8" width="61.83203125" style="9" customWidth="1"/>
+    <col min="9" max="9" width="34.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" style="9" customWidth="1"/>
+    <col min="11" max="11" width="15.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5" style="9" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.83203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="37" style="9" bestFit="1" customWidth="1"/>
+    <col min="17" max="16384" width="8.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="26"/>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="25" t="s">
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="14" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26"/>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26"/>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26"/>
-      <c r="N1" s="27"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="15"/>
+      <c r="K1" s="15"/>
+      <c r="L1" s="15"/>
+      <c r="M1" s="15"/>
+      <c r="N1" s="16"/>
     </row>
     <row r="2" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="28" t="s">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="28" t="s">
+      <c r="C2" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="28" t="s">
+      <c r="D2" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="28" t="s">
+      <c r="F2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="28" t="s">
+      <c r="G2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="28" t="s">
+      <c r="H2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="J2" s="28" t="s">
+      <c r="J2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="28" t="s">
+      <c r="K2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="L2" s="28" t="s">
+      <c r="L2" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="M2" s="28" t="s">
+      <c r="M2" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="28" t="s">
+      <c r="N2" s="13" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D3" s="10">
         <v>40</v>
       </c>
-      <c r="E3" s="22">
+      <c r="E3" s="10">
         <v>1</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="G3" s="23" t="s">
+      <c r="G3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="22"/>
-      <c r="J3" s="23"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
+      <c r="I3" s="10"/>
+      <c r="J3" s="11"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
     </row>
     <row r="4" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="23" t="s">
+      <c r="A4" s="10"/>
+      <c r="B4" s="10"/>
+      <c r="C4" s="10"/>
+      <c r="D4" s="10"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I4" s="23"/>
-      <c r="J4" s="23"/>
-      <c r="K4" s="23"/>
-      <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-      <c r="N4" s="23"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="23" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="10"/>
+      <c r="C5" s="10"/>
+      <c r="D5" s="10"/>
+      <c r="E5" s="10"/>
+      <c r="F5" s="10"/>
+      <c r="G5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="22"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
+      <c r="I5" s="10"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="23" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="10"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="10"/>
+      <c r="G6" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="22"/>
-      <c r="D7" s="22"/>
-      <c r="E7" s="22"/>
-      <c r="F7" s="22"/>
-      <c r="G7" s="23" t="s">
+      <c r="A7" s="10"/>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="22"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="22" t="s">
+      <c r="A8" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D8" s="10">
         <v>20</v>
       </c>
-      <c r="E8" s="22">
+      <c r="E8" s="10">
         <v>1</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="G8" s="23" t="s">
+      <c r="G8" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="22"/>
-      <c r="J8" s="23"/>
-      <c r="K8" s="23"/>
-      <c r="L8" s="23"/>
-      <c r="M8" s="23"/>
-      <c r="N8" s="23"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="22"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="22"/>
-      <c r="D9" s="22"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23" t="s">
+      <c r="A9" s="10"/>
+      <c r="B9" s="10"/>
+      <c r="C9" s="10"/>
+      <c r="D9" s="10"/>
+      <c r="E9" s="10"/>
+      <c r="F9" s="10"/>
+      <c r="G9" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="22"/>
-      <c r="J9" s="23"/>
-      <c r="K9" s="23"/>
-      <c r="L9" s="23"/>
-      <c r="M9" s="23"/>
-      <c r="N9" s="23"/>
-      <c r="O9" s="24"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="11"/>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11"/>
+      <c r="M9" s="11"/>
+      <c r="N9" s="11"/>
+      <c r="O9" s="12"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="22"/>
-      <c r="B10" s="22"/>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
-      <c r="F10" s="22"/>
-      <c r="G10" s="23" t="s">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="10"/>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="23"/>
-      <c r="J10" s="23"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="23"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="22"/>
-      <c r="B11" s="22"/>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="23" t="s">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10"/>
+      <c r="C11" s="10"/>
+      <c r="D11" s="10"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="23"/>
-      <c r="J11" s="23"/>
-      <c r="K11" s="23"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11"/>
+      <c r="N11" s="11"/>
     </row>
     <row r="12" spans="1:15" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="22" t="s">
+      <c r="A12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="22">
+      <c r="D12" s="10">
         <v>20</v>
       </c>
-      <c r="E12" s="22">
+      <c r="E12" s="10">
         <v>2</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="23"/>
-      <c r="J12" s="23"/>
-      <c r="K12" s="23"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="11"/>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
     </row>
     <row r="13" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="22"/>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="23" t="s">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+      <c r="D13" s="10"/>
+      <c r="E13" s="10"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="23" t="s">
+      <c r="I13" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="23" t="s">
+      <c r="K13" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="N13" s="22" t="s">
+      <c r="N13" s="10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="22"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="23" t="s">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="10"/>
+      <c r="F14" s="10"/>
+      <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="I14" s="23"/>
-      <c r="J14" s="23"/>
-      <c r="K14" s="23"/>
-      <c r="L14" s="23"/>
-      <c r="M14" s="23"/>
-      <c r="N14" s="23"/>
+      <c r="I14" s="11"/>
+      <c r="J14" s="11"/>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11"/>
+      <c r="M14" s="11"/>
+      <c r="N14" s="11"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
@@ -1239,12 +1239,12 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="14"/>
+      <c r="B3" s="20"/>
+      <c r="C3" s="20"/>
+      <c r="D3" s="21"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
@@ -1295,10 +1295,10 @@
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
+      <c r="A8" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B8" s="10" t="s">
+      <c r="B8" s="22" t="s">
         <v>46</v>
       </c>
       <c r="C8" s="1" t="s">
@@ -1307,8 +1307,8 @@
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" ht="60" x14ac:dyDescent="0.2">
-      <c r="A9" s="16"/>
-      <c r="B9" s="11"/>
+      <c r="A9" s="28"/>
+      <c r="B9" s="23"/>
       <c r="C9" s="1" t="s">
         <v>45</v>
       </c>
@@ -1345,39 +1345,39 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="14"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="20"/>
+      <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="B13" s="15"/>
-      <c r="C13" s="15"/>
-      <c r="D13" s="15"/>
+      <c r="B13" s="24"/>
+      <c r="C13" s="24"/>
+      <c r="D13" s="24"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="B14" s="8"/>
-      <c r="C14" s="8"/>
-      <c r="D14" s="9"/>
+      <c r="B14" s="26"/>
+      <c r="C14" s="26"/>
+      <c r="D14" s="27"/>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="7">
+    <mergeCell ref="A14:D14"/>
+    <mergeCell ref="A8:A9"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A3:D3"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A14:D14"/>
-    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1397,32 +1397,32 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19" t="s">
+      <c r="A1" s="7" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="7" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="7" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="8" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="8" t="s">
         <v>62</v>
       </c>
     </row>

</xml_diff>